<commit_message>
Added the Contact Page
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\POMBasics\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3529F832-64DE-4E22-846E-71126A27E8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F943A779-021C-4523-A391-D886FEB40B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
     <sheet name="AddAccountTestRCRM" sheetId="7" r:id="rId3"/>
-    <sheet name="LoginTest" sheetId="1" r:id="rId4"/>
-    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId5"/>
-    <sheet name="createAccountTest" sheetId="4" r:id="rId6"/>
+    <sheet name="CreateContactTestReallyCRM" sheetId="8" r:id="rId4"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId5"/>
+    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId6"/>
+    <sheet name="createAccountTest" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>TCID</t>
   </si>
@@ -123,6 +124,78 @@
   </si>
   <si>
     <t>Banking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first </t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>assistant</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>localaddress</t>
+  </si>
+  <si>
+    <t>localcity</t>
+  </si>
+  <si>
+    <t>localzip</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>kanti</t>
+  </si>
+  <si>
+    <t>dutta</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>a@gmail.com</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>CreateContactTestReallyCRM</t>
+  </si>
+  <si>
+    <t>toma</t>
+  </si>
+  <si>
+    <t>beula st</t>
+  </si>
+  <si>
+    <t>new york</t>
   </si>
 </sst>
 </file>
@@ -451,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,6 +556,14 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -529,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998AEEBC-8A86-4DE7-94C8-35C197F5BFB5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -607,6 +688,117 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65400F54-90CA-4032-AB6B-C89A99533987}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="15.26953125" customWidth="1"/>
+    <col min="11" max="11" width="12.90625" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2">
+        <v>12345</v>
+      </c>
+      <c r="H2">
+        <v>4567</v>
+      </c>
+      <c r="I2">
+        <v>6544</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2">
+        <v>22345</v>
+      </c>
+      <c r="N2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{E18B5DF5-9741-4BD0-B12C-1CCFD5B202AA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -647,7 +839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD3A80F-89E0-4436-B269-DA62DD5BC497}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -688,7 +880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Opportunity section is added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\POMBasics\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F943A779-021C-4523-A391-D886FEB40B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C46B343-B9D3-450A-AF14-9126D4FA246C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
-    <sheet name="AddAccountTestRCRM" sheetId="7" r:id="rId3"/>
-    <sheet name="CreateContactTestReallyCRM" sheetId="8" r:id="rId4"/>
-    <sheet name="LoginTest" sheetId="1" r:id="rId5"/>
-    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId6"/>
-    <sheet name="createAccountTest" sheetId="4" r:id="rId7"/>
+    <sheet name="OpportunityTestRCRM" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="AddAccountTestRCRM" sheetId="7" r:id="rId4"/>
+    <sheet name="CreateContactTestRCRM" sheetId="8" r:id="rId5"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId6"/>
+    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId7"/>
+    <sheet name="createAccountTest" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>TCID</t>
   </si>
@@ -186,9 +187,6 @@
     <t>Congo</t>
   </si>
   <si>
-    <t>CreateContactTestReallyCRM</t>
-  </si>
-  <si>
     <t>toma</t>
   </si>
   <si>
@@ -196,6 +194,27 @@
   </si>
   <si>
     <t>new york</t>
+  </si>
+  <si>
+    <t>OpportunityTestRCRM</t>
+  </si>
+  <si>
+    <t>oppName</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>nxtStep</t>
+  </si>
+  <si>
+    <t>competitor</t>
+  </si>
+  <si>
+    <t>acname</t>
+  </si>
+  <si>
+    <t>Lucky2</t>
   </si>
 </sst>
 </file>
@@ -527,12 +546,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -561,7 +580,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -573,11 +592,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74B5B09-858F-4DFF-91B4-2EB0D1E5F8F5}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB78087-F65E-42F6-AFB4-F8E8CA9C6E11}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74B5B09-858F-4DFF-91B4-2EB0D1E5F8F5}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,7 +651,7 @@
     <col min="1" max="1" width="16.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -593,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -601,17 +667,118 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>12345</v>
+      </c>
+      <c r="E6">
+        <v>4567</v>
+      </c>
+      <c r="F6">
+        <v>6544</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6">
+        <v>22345</v>
+      </c>
+      <c r="K6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{E18B5DF5-9741-4BD0-B12C-1CCFD5B202AA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998AEEBC-8A86-4DE7-94C8-35C197F5BFB5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,7 +818,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -687,12 +854,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65400F54-90CA-4032-AB6B-C89A99533987}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,108 +869,27 @@
     <col min="12" max="12" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2">
-        <v>12345</v>
-      </c>
-      <c r="H2">
-        <v>4567</v>
-      </c>
-      <c r="I2">
-        <v>6544</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2">
-        <v>22345</v>
-      </c>
-      <c r="N2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{E18B5DF5-9741-4BD0-B12C-1CCFD5B202AA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -839,7 +925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD3A80F-89E0-4436-B269-DA62DD5BC497}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -880,7 +966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Flow Lu Crm Opportunities is added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\POMBasics\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C46B343-B9D3-450A-AF14-9126D4FA246C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBDEA79-EAE6-47A8-A392-1893F775DB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="OpportunityTestRCRM" sheetId="9" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="AddAccountTestRCRM" sheetId="7" r:id="rId4"/>
-    <sheet name="CreateContactTestRCRM" sheetId="8" r:id="rId5"/>
-    <sheet name="LoginTest" sheetId="1" r:id="rId6"/>
-    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId7"/>
-    <sheet name="createAccountTest" sheetId="4" r:id="rId8"/>
+    <sheet name="AddOpportunityTestFlow" sheetId="11" r:id="rId2"/>
+    <sheet name="LoginTestFlow" sheetId="10" r:id="rId3"/>
+    <sheet name="OpportunityTestRCRM" sheetId="9" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="AddAccountTestRCRM" sheetId="7" r:id="rId6"/>
+    <sheet name="CreateContactTestRCRM" sheetId="8" r:id="rId7"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId8"/>
+    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId9"/>
+    <sheet name="createAccountTest" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>TCID</t>
   </si>
@@ -215,6 +217,36 @@
   </si>
   <si>
     <t>Lucky2</t>
+  </si>
+  <si>
+    <t>LoginTestFlow</t>
+  </si>
+  <si>
+    <t>AddOpportunityTestFlow</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>oraganization</t>
+  </si>
+  <si>
+    <t>contactperson</t>
+  </si>
+  <si>
+    <t>iskcon</t>
+  </si>
+  <si>
+    <t>bluetoothprabu</t>
   </si>
 </sst>
 </file>
@@ -543,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,7 +596,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -572,17 +604,9 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -591,7 +615,143 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BBCB55-59F4-47EF-9048-F43A81BEFECB}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2">
+        <v>900000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0C43F6A2-6593-43B6-ADB9-8CD9C054653C}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{0AA5D98C-1D47-49F5-9AB1-B20378DC6CB5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904CB4FC-8D8D-461C-B272-4B9D453999AC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AE200BEE-0B95-4650-89DD-D811A72A3CA5}"/>
+    <hyperlink ref="B2" r:id="rId2" display="Selenium@123" xr:uid="{2DC7CA55-5D99-4146-8B52-769CB63EBBD8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB78087-F65E-42F6-AFB4-F8E8CA9C6E11}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -638,12 +798,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74B5B09-858F-4DFF-91B4-2EB0D1E5F8F5}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,6 +925,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" xr:uid="{E18B5DF5-9741-4BD0-B12C-1CCFD5B202AA}"/>
@@ -773,11 +965,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998AEEBC-8A86-4DE7-94C8-35C197F5BFB5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -854,7 +1046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65400F54-90CA-4032-AB6B-C89A99533987}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -884,12 +1076,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,7 +1117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD3A80F-89E0-4436-B269-DA62DD5BC497}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -964,27 +1156,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
New Contact Page is added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\POMBasics\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDA4C1-842F-47BF-AE80-5CC61845B4A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E14399-96CA-465D-BFA1-33E90982C32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="AddOpportunityTestFlow" sheetId="11" r:id="rId2"/>
     <sheet name="AddOrganizationTestFlow" sheetId="12" r:id="rId3"/>
-    <sheet name="LoginTestFlow" sheetId="10" r:id="rId4"/>
-    <sheet name="OpportunityTestRCRM" sheetId="9" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
-    <sheet name="AddAccountTestRCRM" sheetId="7" r:id="rId7"/>
-    <sheet name="CreateContactTestRCRM" sheetId="8" r:id="rId8"/>
-    <sheet name="LoginTest" sheetId="1" r:id="rId9"/>
-    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId10"/>
-    <sheet name="createAccountTest" sheetId="4" r:id="rId11"/>
+    <sheet name="AddNewContactTest" sheetId="13" r:id="rId4"/>
+    <sheet name="LoginTestFlow" sheetId="10" r:id="rId5"/>
+    <sheet name="OpportunityTestRCRM" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId7"/>
+    <sheet name="AddAccountTestRCRM" sheetId="7" r:id="rId8"/>
+    <sheet name="CreateContactTestRCRM" sheetId="8" r:id="rId9"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId10"/>
+    <sheet name="LoginTestReallyCRM" sheetId="5" r:id="rId11"/>
+    <sheet name="createAccountTest" sheetId="4" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>TCID</t>
   </si>
@@ -275,6 +276,12 @@
   </si>
   <si>
     <t>A@gmail.com</t>
+  </si>
+  <si>
+    <t>Om</t>
+  </si>
+  <si>
+    <t>AddNewContactTest</t>
   </si>
 </sst>
 </file>
@@ -603,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,12 +653,61 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="Selenium@123" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD3A80F-89E0-4436-B269-DA62DD5BC497}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -692,7 +748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -791,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47AAF56-450E-48AB-8628-91D500C4BD8E}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -859,6 +915,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F260ED-6980-4161-B69D-0A70FD460C86}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904CB4FC-8D8D-461C-B272-4B9D453999AC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -899,7 +980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB78087-F65E-42F6-AFB4-F8E8CA9C6E11}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -946,7 +1027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74B5B09-858F-4DFF-91B4-2EB0D1E5F8F5}">
   <dimension ref="A1:M13"/>
   <sheetViews>
@@ -1113,7 +1194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998AEEBC-8A86-4DE7-94C8-35C197F5BFB5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1194,7 +1275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65400F54-90CA-4032-AB6B-C89A99533987}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1222,45 +1303,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="Selenium@123" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>